<commit_message>
updated to use pd.Intervals for ls code
</commit_message>
<xml_diff>
--- a/templates/tb.xlsx
+++ b/templates/tb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="format1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t xml:space="preserve">Account No </t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>None</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Assets - Current - trade receivable</t>
@@ -418,30 +415,30 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,18 +467,18 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1111</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>7200.4009999999998</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -499,15 +496,15 @@
         <v>456</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2222</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>3000.1</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -528,18 +525,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3333</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>5650.1</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>-33434</v>
@@ -557,18 +554,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4444</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>7200.4</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>432</v>
@@ -586,18 +583,18 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5555</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4">
         <v>7420</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="4">
         <v>2320</v>
@@ -615,18 +612,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>5200</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -644,12 +641,12 @@
         <v>12303</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2">
         <v>6300.2</v>

</xml_diff>